<commit_message>
Adding windows PS directory/file metadata harvesting script, adding initial DB design as I think the best method for storing and referencing this data is SqlLite. Adding start of Python script to update the DB with the metadata.
</commit_message>
<xml_diff>
--- a/DB_design.xlsx
+++ b/DB_design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flakes/code/OS-defaults_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103C4E4A-FCF4-F34D-AEC2-16B7E12540D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B1F06D-FA5D-ED44-8E3A-A33A97A4F8D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22000" yWindow="560" windowWidth="25920" windowHeight="17580" xr2:uid="{117B77E5-A4A7-F24D-B575-B104BEDDAD89}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="20220" windowHeight="14680" xr2:uid="{117B77E5-A4A7-F24D-B575-B104BEDDAD89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Table</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Link</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>os_id</t>
   </si>
   <si>
@@ -115,6 +112,15 @@
   </si>
   <si>
     <t>os_directory_item_id</t>
+  </si>
+  <si>
+    <t>Item_ADS</t>
+  </si>
+  <si>
+    <t>ads_id</t>
+  </si>
+  <si>
+    <t>rowid</t>
   </si>
 </sst>
 </file>
@@ -138,7 +144,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +163,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -170,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -178,6 +190,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5A86AD-5B74-814A-9964-C48F4D00269A}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -507,9 +520,10 @@
     <col min="5" max="5" width="15.5" customWidth="1"/>
     <col min="6" max="6" width="20.83203125" customWidth="1"/>
     <col min="7" max="8" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -523,141 +537,150 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
       <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="F6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="F7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="F8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
building out DB Python import
</commit_message>
<xml_diff>
--- a/DB_design.xlsx
+++ b/DB_design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flakes/code/OS-defaults_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B1F06D-FA5D-ED44-8E3A-A33A97A4F8D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C522F9-CDC8-9E49-9D9A-1A06230C90FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="500" windowWidth="20220" windowHeight="14680" xr2:uid="{117B77E5-A4A7-F24D-B575-B104BEDDAD89}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Table</t>
   </si>
@@ -54,6 +54,9 @@
     <t>Link</t>
   </si>
   <si>
+    <t>id</t>
+  </si>
+  <si>
     <t>os_id</t>
   </si>
   <si>
@@ -120,7 +123,7 @@
     <t>ads_id</t>
   </si>
   <si>
-    <t>rowid</t>
+    <t>bits</t>
   </si>
 </sst>
 </file>
@@ -508,7 +511,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,19 +540,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -557,106 +560,109 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Building out Python script for harvesting Mac and Linux defaults. Added 'Hidden' field to track that seperately.
</commit_message>
<xml_diff>
--- a/DB_design.xlsx
+++ b/DB_design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flakes/code/OS-defaults_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C522F9-CDC8-9E49-9D9A-1A06230C90FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B75F90-3CE0-1346-A5BA-C71796CA136C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="20220" windowHeight="14680" xr2:uid="{117B77E5-A4A7-F24D-B575-B104BEDDAD89}"/>
+    <workbookView xWindow="43780" yWindow="500" windowWidth="20220" windowHeight="14680" xr2:uid="{117B77E5-A4A7-F24D-B575-B104BEDDAD89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Table</t>
   </si>
@@ -63,9 +63,6 @@
     <t>directory_id</t>
   </si>
   <si>
-    <t>file_id</t>
-  </si>
-  <si>
     <t>arch</t>
   </si>
   <si>
@@ -108,7 +105,7 @@
     <t>link_id</t>
   </si>
   <si>
-    <t>link_target_id</t>
+    <t>item_id</t>
   </si>
   <si>
     <t>OS_Directory_Item</t>
@@ -124,6 +121,12 @@
   </si>
   <si>
     <t>bits</t>
+  </si>
+  <si>
+    <t>target_id</t>
+  </si>
+  <si>
+    <t>hidden</t>
   </si>
 </sst>
 </file>
@@ -511,7 +514,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,19 +543,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -587,86 +590,89 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
       <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>

</xml_diff>

<commit_message>
adding more fields and updating DB structure.
</commit_message>
<xml_diff>
--- a/DB_design.xlsx
+++ b/DB_design.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flakes/code/OS-defaults_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276B9A96-133C-B24E-A23A-E9FB4BCB0E67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10286B40-34EE-C54D-9AE0-772FB102D6EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43780" yWindow="500" windowWidth="20220" windowHeight="14680" xr2:uid="{117B77E5-A4A7-F24D-B575-B104BEDDAD89}"/>
+    <workbookView xWindow="39420" yWindow="500" windowWidth="24580" windowHeight="22960" xr2:uid="{117B77E5-A4A7-F24D-B575-B104BEDDAD89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
   <si>
     <t>Table</t>
   </si>
@@ -127,6 +127,99 @@
   </si>
   <si>
     <t>is_hidden</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>company_name</t>
+  </si>
+  <si>
+    <t>file_build_part</t>
+  </si>
+  <si>
+    <t>file_description</t>
+  </si>
+  <si>
+    <t>file_major_part</t>
+  </si>
+  <si>
+    <t>file_minor_part</t>
+  </si>
+  <si>
+    <t>file_private_part</t>
+  </si>
+  <si>
+    <t>file_version</t>
+  </si>
+  <si>
+    <t>internal_name</t>
+  </si>
+  <si>
+    <t>is_debug</t>
+  </si>
+  <si>
+    <t>is_patched</t>
+  </si>
+  <si>
+    <t>is_private_build</t>
+  </si>
+  <si>
+    <t>is_prerelease</t>
+  </si>
+  <si>
+    <t>is_special_build</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>legal_copyright</t>
+  </si>
+  <si>
+    <t>legal_trademarks</t>
+  </si>
+  <si>
+    <t>original_filename</t>
+  </si>
+  <si>
+    <t>filename</t>
+  </si>
+  <si>
+    <t>private_build</t>
+  </si>
+  <si>
+    <t>product_build_part</t>
+  </si>
+  <si>
+    <t>product_major_part</t>
+  </si>
+  <si>
+    <t>product_minor_part</t>
+  </si>
+  <si>
+    <t>product_name</t>
+  </si>
+  <si>
+    <t>product_private_part</t>
+  </si>
+  <si>
+    <t>product_version</t>
+  </si>
+  <si>
+    <t>md5</t>
+  </si>
+  <si>
+    <t>sha1</t>
+  </si>
+  <si>
+    <t>sha256</t>
+  </si>
+  <si>
+    <t>Hash</t>
+  </si>
+  <si>
+    <t>hash_id</t>
   </si>
 </sst>
 </file>
@@ -511,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5A86AD-5B74-814A-9964-C48F4D00269A}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -529,7 +622,7 @@
     <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,8 +650,11 @@
       <c r="I1" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -586,8 +682,11 @@
       <c r="I2" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" t="s">
         <v>9</v>
@@ -613,8 +712,11 @@
       <c r="I3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>27</v>
@@ -634,8 +736,11 @@
       <c r="I4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="C5" t="s">
         <v>12</v>
@@ -649,78 +754,184 @@
       <c r="I5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="F6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="F7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="F8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="F9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="F10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
+      <c r="F25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F36" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added group and user metadata; windows is hacked in that I can't tell if thw owner is a group or user yet
</commit_message>
<xml_diff>
--- a/DB_design.xlsx
+++ b/DB_design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flakes/code/OS-defaults_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2284B52-1658-FF40-973C-680368A3F13C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8133D5D0-310B-3B47-93E4-A7656B759A98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39420" yWindow="500" windowWidth="24580" windowHeight="22960" xr2:uid="{117B77E5-A4A7-F24D-B575-B104BEDDAD89}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
   <si>
     <t>Table</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>OS_Directory_Item_Hash</t>
+  </si>
+  <si>
+    <t>Group_User</t>
   </si>
 </sst>
 </file>
@@ -604,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5A86AD-5B74-814A-9964-C48F4D00269A}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,7 +625,7 @@
     <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,8 +656,11 @@
       <c r="J1" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -685,8 +691,11 @@
       <c r="J2" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" t="s">
         <v>9</v>
@@ -715,8 +724,11 @@
       <c r="J3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>26</v>
@@ -740,7 +752,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="C5" t="s">
         <v>12</v>
@@ -758,67 +770,67 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="F6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="F7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="F8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="F9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="F10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="F11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="F12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="F13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="F14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="F15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="F16" t="s">
         <v>35</v>

</xml_diff>